<commit_message>
map2, call static method occur compile error, WTF?
</commit_message>
<xml_diff>
--- a/excel/工作簿3.xlsx
+++ b/excel/工作簿3.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Project\magic-tower\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="2" r:id="rId1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="145">
   <si>
     <t>monster</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,11 +349,75 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>specail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>specail</t>
+    <t>sprite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>door-yellow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>door-blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>door-red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>door-specail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key-yellow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key-blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key-red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key-yellow,key-blue,key-red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stairs-up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>减少道具后自毁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动地图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEXT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stairs-down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PREVIOUS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fence</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -366,75 +425,139 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>change_map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defeat_monster_to_destroy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>star</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sword-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheild-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheild-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheild-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheild-4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sheild-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sprite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阻碍移动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>door-yellow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>door-blue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>door-red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>door-specail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key-yellow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key-blue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key-red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>key-yellow,key-blue,key-red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stairs-up</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>减少道具后自毁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动地图</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEXT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stairs-down</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PREVIOUS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fence</t>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>npc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>robot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>158,159</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>busineesman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>160,161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oldman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>162,163</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thief</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>164,165</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>princess</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>166,167</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -442,171 +565,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>change_map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>defeat_monster_to_destroy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>block</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>magma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>star</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>add_hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_atk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>add_yellow_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add_blue_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sword-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sword-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sword-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sword-4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sword-5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sheild-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sheild-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sheild-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sheild-4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sheild-5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sprite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>def</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>npc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>robot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>158,159</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>busineesman</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>160,161</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>oldman</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>162,163</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>thief</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>164,165</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>princess</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>166,167</t>
+    <t>add_red_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>item</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -651,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,9 +654,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1004,18 +1002,18 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -1023,7 +1021,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -1031,7 +1029,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -1058,22 +1056,22 @@
       <selection sqref="A1:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.625" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1"/>
-    <col min="4" max="4" width="9.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1"/>
+    <col min="4" max="4" width="9.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1084,16 +1082,16 @@
         <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1104,20 +1102,20 @@
         <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1126,7 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -1137,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1149,7 +1147,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1159,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1173,7 +1171,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1183,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1197,7 +1195,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +1207,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1221,7 +1219,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1231,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1245,7 +1243,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1257,7 +1255,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1269,7 +1267,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1281,7 +1279,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1293,7 +1291,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1305,7 +1303,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1315,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1329,7 +1327,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1341,7 +1339,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1353,7 +1351,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1365,7 +1363,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1377,7 +1375,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1389,7 +1387,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1399,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1413,7 +1411,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1425,7 +1423,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1437,7 +1435,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1449,7 +1447,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1461,7 +1459,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1474,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1489,24 +1487,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1517,7 +1515,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1528,182 +1526,182 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1">
         <v>158</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B6" s="1">
         <v>160</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B7" s="1">
         <v>162</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1">
         <v>164</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B9" s="1">
         <v>166</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
@@ -1711,35 +1709,39 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="31.875" customWidth="1"/>
-    <col min="7" max="7" width="28.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -1747,22 +1749,19 @@
         <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1770,33 +1769,27 @@
         <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="D4" s="1" t="s">
-        <v>86</v>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="D4" t="s">
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -1806,13 +1799,10 @@
       <c r="C5" s="1">
         <v>68</v>
       </c>
-      <c r="D5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1">
         <v>67</v>
@@ -1820,16 +1810,13 @@
       <c r="C6" s="1">
         <v>67</v>
       </c>
-      <c r="D6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B7" s="1">
         <v>66</v>
@@ -1837,16 +1824,13 @@
       <c r="C7" s="1">
         <v>66</v>
       </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1">
         <v>65</v>
@@ -1854,16 +1838,13 @@
       <c r="C8" s="1">
         <v>65</v>
       </c>
-      <c r="D8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1">
         <v>64</v>
@@ -1871,16 +1852,13 @@
       <c r="C9" s="1">
         <v>64</v>
       </c>
-      <c r="D9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1">
         <v>56</v>
@@ -1888,16 +1866,13 @@
       <c r="C10" s="1">
         <v>56</v>
       </c>
-      <c r="D10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B11" s="1">
         <v>55</v>
@@ -1905,16 +1880,13 @@
       <c r="C11" s="1">
         <v>55</v>
       </c>
-      <c r="D11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="1">
         <v>54</v>
@@ -1922,16 +1894,13 @@
       <c r="C12" s="1">
         <v>54</v>
       </c>
-      <c r="D12" s="1" t="b">
+      <c r="F12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B13" s="1">
         <v>50</v>
@@ -1939,52 +1908,54 @@
       <c r="C13" s="1">
         <v>50</v>
       </c>
-      <c r="D13" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B14" s="1">
         <v>49</v>
       </c>
       <c r="C14" s="1">
         <v>49</v>
-      </c>
-      <c r="D14" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1995,16 +1966,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+        <v>135</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2012,23 +1992,32 @@
         <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -2038,8 +2027,11 @@
       <c r="C5" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>75</v>
       </c>
@@ -2049,8 +2041,11 @@
       <c r="C6" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -2060,8 +2055,11 @@
       <c r="C7" s="1">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>77</v>
       </c>
@@ -2071,8 +2069,11 @@
       <c r="C8" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>78</v>
       </c>
@@ -2082,8 +2083,11 @@
       <c r="C9" s="1">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
@@ -2093,8 +2097,11 @@
       <c r="C10" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
@@ -2104,10 +2111,13 @@
       <c r="C11" s="1">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="D11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B12" s="1">
         <v>46</v>
@@ -2116,9 +2126,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B13" s="1">
         <v>45</v>
@@ -2127,9 +2137,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B14" s="1">
         <v>44</v>
@@ -2138,9 +2148,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B15" s="1">
         <v>43</v>
@@ -2149,9 +2159,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B16" s="1">
         <v>42</v>
@@ -2160,9 +2170,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B17" s="1">
         <v>41</v>
@@ -2171,9 +2181,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B18" s="1">
         <v>40</v>
@@ -2182,9 +2192,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B19" s="1">
         <v>39</v>
@@ -2193,9 +2203,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1">
         <v>38</v>
@@ -2204,9 +2214,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1">
         <v>37</v>
@@ -2218,6 +2228,11 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>